<commit_message>
Getting ADC samples with DMA
</commit_message>
<xml_diff>
--- a/docs/hz.xlsx
+++ b/docs/hz.xlsx
@@ -110,7 +110,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,9 +129,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,10 +681,10 @@
       <c r="G3" s="1"/>
       <c r="H3" s="5">
         <f>(1/I2)*I3</f>
-        <v>2.3833333333333334e-005</v>
+        <v>7.983333333333334e-005</v>
       </c>
       <c r="I3" s="6">
-        <v>71.5</v>
+        <v>239.5</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>2</v>
@@ -718,7 +715,7 @@
       <c r="E5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
@@ -735,14 +732,14 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>4</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="H6">
         <f>1/H3</f>
-        <v>41958.041958041955</v>
+        <v>12526.096033402922</v>
       </c>
       <c r="M6">
         <v>7.5</v>
@@ -753,20 +750,20 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <f>1/B7</f>
+        <f t="shared" ref="C7:C9" si="0">1/B7</f>
         <v>0.20000000000000001</v>
       </c>
       <c r="D7" s="1">
-        <f>C7*$D$6</f>
+        <f t="shared" ref="D7:D9" si="1">C7*$D$6</f>
         <v>0.80000000000000004</v>
       </c>
-      <c r="E7" s="10">
-        <f>ROUNDDOWN(C7/$H$3,0)</f>
-        <v>8391</v>
-      </c>
-      <c r="F7" s="11">
-        <f>E7*$D$6</f>
-        <v>33564</v>
+      <c r="E7" s="9">
+        <f t="shared" ref="E7:E9" si="2">ROUNDDOWN(C7/$H$3,0)</f>
+        <v>2505</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" ref="F7:F9" si="3">E7*$D$6</f>
+        <v>10020</v>
       </c>
       <c r="M7">
         <v>13.5</v>
@@ -777,20 +774,20 @@
         <v>10</v>
       </c>
       <c r="C8" s="1">
-        <f>1/B8</f>
+        <f t="shared" si="0"/>
         <v>0.10000000000000001</v>
       </c>
       <c r="D8" s="1">
-        <f>C8*$D$6</f>
+        <f t="shared" si="1"/>
         <v>0.40000000000000002</v>
       </c>
-      <c r="E8" s="10">
-        <f>ROUNDDOWN(C8/$H$3,0)</f>
-        <v>4195</v>
-      </c>
-      <c r="F8" s="11">
-        <f>E8*$D$6</f>
-        <v>16780</v>
+      <c r="E8" s="9">
+        <f t="shared" si="2"/>
+        <v>1252</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="3"/>
+        <v>5008</v>
       </c>
       <c r="M8">
         <v>28.5</v>
@@ -801,20 +798,20 @@
         <v>50</v>
       </c>
       <c r="C9" s="1">
-        <f>1/B9</f>
+        <f t="shared" si="0"/>
         <v>2.e-002</v>
       </c>
       <c r="D9" s="1">
-        <f>C9*$D$6</f>
+        <f t="shared" si="1"/>
         <v>8.0000000000000002e-002</v>
       </c>
-      <c r="E9" s="10">
-        <f>ROUNDDOWN(C9/$H$3,0)</f>
-        <v>839</v>
-      </c>
-      <c r="F9" s="11">
-        <f>E9*$D$6</f>
-        <v>3356</v>
+      <c r="E9" s="9">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="3"/>
+        <v>1000</v>
       </c>
       <c r="M9">
         <v>41.5</v>
@@ -825,20 +822,20 @@
         <v>100</v>
       </c>
       <c r="C10" s="1">
-        <f>1/B10</f>
+        <f t="shared" ref="C10:C12" si="4">1/B10</f>
         <v>1.e-002</v>
       </c>
       <c r="D10" s="1">
-        <f>C10*$D$6</f>
+        <f t="shared" ref="D10:D12" si="5">C10*$D$6</f>
         <v>4.0000000000000001e-002</v>
       </c>
-      <c r="E10" s="10">
-        <f>ROUNDDOWN(C10/$H$3,0)</f>
-        <v>419</v>
-      </c>
-      <c r="F10" s="11">
-        <f>E10*$D$6</f>
-        <v>1676</v>
+      <c r="E10" s="9">
+        <f t="shared" ref="E10:E12" si="6">ROUNDDOWN(C10/$H$3,0)</f>
+        <v>125</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" ref="F10:F12" si="7">E10*$D$6</f>
+        <v>500</v>
       </c>
       <c r="M10">
         <v>55.5</v>
@@ -849,20 +846,20 @@
         <v>200</v>
       </c>
       <c r="C11" s="1">
-        <f>1/B11</f>
+        <f t="shared" si="4"/>
         <v>5.0000000000000001e-003</v>
       </c>
       <c r="D11" s="1">
-        <f>C11*$D$6</f>
+        <f t="shared" si="5"/>
         <v>2.e-002</v>
       </c>
-      <c r="E11" s="10">
-        <f>ROUNDDOWN(C11/$H$3,0)</f>
-        <v>209</v>
-      </c>
-      <c r="F11" s="11">
-        <f>E11*$D$6</f>
-        <v>836</v>
+      <c r="E11" s="9">
+        <f t="shared" si="6"/>
+        <v>62</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="7"/>
+        <v>248</v>
       </c>
       <c r="M11">
         <v>71.5</v>
@@ -873,20 +870,20 @@
         <v>500</v>
       </c>
       <c r="C12" s="1">
-        <f>1/B12</f>
+        <f t="shared" si="4"/>
         <v>2.e-003</v>
       </c>
       <c r="D12" s="1">
-        <f>C12*$D$6</f>
+        <f t="shared" si="5"/>
         <v>8.0000000000000002e-003</v>
       </c>
-      <c r="E12" s="10">
-        <f>ROUNDDOWN(C12/$H$3,0)</f>
-        <v>83</v>
-      </c>
-      <c r="F12" s="11">
-        <f>E12*$D$6</f>
-        <v>332</v>
+      <c r="E12" s="9">
+        <f t="shared" si="6"/>
+        <v>25</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="7"/>
+        <v>100</v>
       </c>
       <c r="M12">
         <v>239.5</v>
@@ -897,7 +894,7 @@
         <v>72000000</v>
       </c>
       <c r="I16">
-        <f>1/H16</f>
+        <f t="shared" ref="I16:I17" si="8">1/H16</f>
         <v>1.3888888888888889e-008</v>
       </c>
     </row>
@@ -907,7 +904,7 @@
         <v>20000</v>
       </c>
       <c r="I17">
-        <f>1/H17</f>
+        <f t="shared" si="8"/>
         <v>5.0000000000000002e-005</v>
       </c>
     </row>

</xml_diff>